<commit_message>
Before adding blended capability
</commit_message>
<xml_diff>
--- a/results/Xr_Results.xlsx
+++ b/results/Xr_Results.xlsx
@@ -256,28 +256,28 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D7">
-        <v>3990</v>
+        <v>4401</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>7</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>4023</v>
+        <v>4401</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>7</v>
       </c>
       <c r="K7">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="L7">
-        <v>4839</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -285,28 +285,28 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <v>4994</v>
+        <v>4233</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>8</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>5000</v>
+        <v>4306</v>
       </c>
       <c r="J8" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K8">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="L8">
-        <v>5000</v>
+        <v>4864</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -325,19 +325,19 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>0.09702380952380953</v>
+        <v>0.08988095238095238</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>7</v>
       </c>
       <c r="G11">
-        <v>0.0011904761904761906</v>
+        <v>0.0</v>
       </c>
       <c r="J11" t="s" s="0">
         <v>7</v>
       </c>
       <c r="K11">
-        <v>0.11822660098522167</v>
+        <v>0.08374384236453201</v>
       </c>
     </row>
     <row r="12" spans="2:12">
@@ -345,19 +345,19 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>0.029166666666666667</v>
+        <v>0.039285714285714285</v>
       </c>
       <c r="F12" t="s" s="0">
         <v>8</v>
       </c>
       <c r="G12">
-        <v>0.0011904761904761906</v>
+        <v>0.0</v>
       </c>
       <c r="J12" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K12">
-        <v>0.025123152709359605</v>
+        <v>0.04039408866995074</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -432,28 +432,28 @@
         <v>7</v>
       </c>
       <c r="C18">
-        <v>157</v>
+        <v>106</v>
       </c>
       <c r="D18">
-        <v>4874</v>
+        <v>4995</v>
       </c>
       <c r="F18" t="s" s="0">
         <v>7</v>
       </c>
       <c r="G18">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="H18">
-        <v>4937</v>
+        <v>4620</v>
       </c>
       <c r="J18" t="s" s="0">
         <v>7</v>
       </c>
       <c r="K18">
-        <v>656</v>
+        <v>503</v>
       </c>
       <c r="L18">
-        <v>22663</v>
+        <v>23297</v>
       </c>
     </row>
     <row r="19" spans="2:12">
@@ -461,28 +461,28 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D19">
-        <v>5000</v>
+        <v>4996</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>8</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="H19">
-        <v>5000</v>
+        <v>4371</v>
       </c>
       <c r="J19" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K19">
-        <v>148</v>
+        <v>293</v>
       </c>
       <c r="L19">
-        <v>24994</v>
+        <v>22770</v>
       </c>
     </row>
     <row r="21" spans="2:12">
@@ -501,19 +501,19 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>0.09090909090909091</v>
+        <v>0.061378112333526344</v>
       </c>
       <c r="F22" t="s" s="0">
         <v>7</v>
       </c>
       <c r="G22">
-        <v>0.3197278911564626</v>
+        <v>0.2585034013605442</v>
       </c>
       <c r="J22" t="s" s="0">
         <v>7</v>
       </c>
       <c r="K22">
-        <v>0.11446518932123538</v>
+        <v>0.08776827778747165</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -521,19 +521,19 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0.016213086276780544</v>
+        <v>0.04400694846554719</v>
       </c>
       <c r="F23" t="s" s="0">
         <v>8</v>
       </c>
       <c r="G23">
-        <v>0.061224489795918366</v>
+        <v>0.23469387755102042</v>
       </c>
       <c r="J23" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K23">
-        <v>0.025824463444425058</v>
+        <v>0.0511254580352469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>